<commit_message>
Changes for report #1
</commit_message>
<xml_diff>
--- a/IT410 Final Project/Data/Download-GDPPC-USD-countries.xlsx
+++ b/IT410 Final Project/Data/Download-GDPPC-USD-countries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\IT410 Final Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D0E596-E935-4713-837E-53185DCD0EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E5203C-22A1-45FD-B92F-44C14EE7D3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17172" windowHeight="8004" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="10956" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Download-GDPPC-USD-countries" sheetId="1" r:id="rId1"/>
@@ -711,7 +711,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -856,6 +856,12 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1201,7 +1207,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1227,6 +1233,14 @@
     </xf>
     <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1582,13 +1596,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AZ221"/>
+  <dimension ref="A1:BA221"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AD41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C13" sqref="C13"/>
       <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
-      <selection pane="bottomRight" activeCell="A44" sqref="A44:XFD46"/>
+      <selection pane="bottomRight" activeCell="C44" sqref="C44:AZ44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1597,7 +1611,9 @@
     <col min="2" max="2" width="30.6640625" style="9" customWidth="1"/>
     <col min="3" max="51" width="8.6640625" style="8" customWidth="1"/>
     <col min="52" max="52" width="9.109375" style="12"/>
-    <col min="53" max="16384" width="9.109375" style="1"/>
+    <col min="53" max="53" width="9.109375" style="1"/>
+    <col min="54" max="54" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -6290,7 +6306,7 @@
         <v>31086.329196002975</v>
       </c>
     </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>100</v>
       </c>
@@ -6448,7 +6464,7 @@
         <v>9703.4878142733378</v>
       </c>
     </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>854</v>
       </c>
@@ -6606,7 +6622,7 @@
         <v>786.8956135895545</v>
       </c>
     </row>
-    <row r="35" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>108</v>
       </c>
@@ -6764,7 +6780,7 @@
         <v>260.3815634109319</v>
       </c>
     </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>132</v>
       </c>
@@ -6922,7 +6938,7 @@
         <v>3603.7825764847412</v>
       </c>
     </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>116</v>
       </c>
@@ -7080,7 +7096,7 @@
         <v>1643.641451311631</v>
       </c>
     </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>120</v>
       </c>
@@ -7238,7 +7254,7 @@
         <v>1501.8082911532936</v>
       </c>
     </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>124</v>
       </c>
@@ -7396,7 +7412,7 @@
         <v>46550.335507365089</v>
       </c>
     </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>136</v>
       </c>
@@ -7554,7 +7570,7 @@
         <v>92692.370523131161</v>
       </c>
     </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>140</v>
       </c>
@@ -7712,7 +7728,7 @@
         <v>467.90724640765944</v>
       </c>
     </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>148</v>
       </c>
@@ -7870,7 +7886,7 @@
         <v>706.82583284397208</v>
       </c>
     </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>152</v>
       </c>
@@ -8028,162 +8044,163 @@
         <v>14896.453866578326</v>
       </c>
     </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:53" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B44" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C44" s="10">
-        <v>1778.6315961735147</v>
-      </c>
-      <c r="D44" s="10">
-        <v>2059.1582732792385</v>
-      </c>
-      <c r="E44" s="10">
-        <v>2549.5830021364627</v>
-      </c>
-      <c r="F44" s="10">
-        <v>3494.6039386123743</v>
-      </c>
-      <c r="G44" s="10">
-        <v>4011.7881437374381</v>
-      </c>
-      <c r="H44" s="10">
-        <v>4402.7375938542618</v>
-      </c>
-      <c r="I44" s="10">
-        <v>4988.9466136581159</v>
-      </c>
-      <c r="J44" s="10">
-        <v>6095.4388190237851</v>
-      </c>
-      <c r="K44" s="10">
-        <v>7347.111147649267</v>
-      </c>
-      <c r="L44" s="10">
-        <v>8594.5620968425173</v>
-      </c>
-      <c r="M44" s="10">
-        <v>10467.839928860047</v>
-      </c>
-      <c r="N44" s="10">
-        <v>10905.155336480784</v>
-      </c>
-      <c r="O44" s="10">
-        <v>11161.297746029439</v>
-      </c>
-      <c r="P44" s="10">
-        <v>10416.042837731326</v>
-      </c>
-      <c r="Q44" s="10">
-        <v>11483.770464911664</v>
-      </c>
-      <c r="R44" s="10">
-        <v>11798.097584837767</v>
-      </c>
-      <c r="S44" s="10">
-        <v>13052.379563477127</v>
-      </c>
-      <c r="T44" s="10">
-        <v>15855.738052869398</v>
-      </c>
-      <c r="U44" s="10">
-        <v>18176.531390878183</v>
-      </c>
-      <c r="V44" s="10">
-        <v>20640.298860478091</v>
-      </c>
-      <c r="W44" s="10">
-        <v>23134.091456904534</v>
-      </c>
-      <c r="X44" s="10">
-        <v>26246.768291846347</v>
-      </c>
-      <c r="Y44" s="10">
-        <v>31654.538598247251</v>
-      </c>
-      <c r="Z44" s="10">
-        <v>36005.554030536834</v>
-      </c>
-      <c r="AA44" s="10">
-        <v>39680.737641142288</v>
-      </c>
-      <c r="AB44" s="10">
-        <v>42514.284179072623</v>
-      </c>
-      <c r="AC44" s="10">
-        <v>44617.452272872324</v>
-      </c>
-      <c r="AD44" s="10">
-        <v>46881.068917362805</v>
-      </c>
-      <c r="AE44" s="10">
-        <v>43587.778426045959</v>
-      </c>
-      <c r="AF44" s="10">
-        <v>41782.188569549311</v>
-      </c>
-      <c r="AG44" s="10">
-        <v>42634.231083423736</v>
-      </c>
-      <c r="AH44" s="10">
-        <v>42001.821579568925</v>
-      </c>
-      <c r="AI44" s="10">
-        <v>42261.746386948027</v>
-      </c>
-      <c r="AJ44" s="10">
-        <v>43070.094517831742</v>
-      </c>
-      <c r="AK44" s="10">
-        <v>48996.288913864424</v>
-      </c>
-      <c r="AL44" s="10">
-        <v>53582.272866498242</v>
-      </c>
-      <c r="AM44" s="10">
-        <v>60459.327410548591</v>
-      </c>
-      <c r="AN44" s="10">
-        <v>69925.985605904498</v>
-      </c>
-      <c r="AO44" s="10">
-        <v>75855.026759155939</v>
-      </c>
-      <c r="AP44" s="10">
-        <v>75456.09414666603</v>
-      </c>
-      <c r="AQ44" s="10">
-        <v>89520.643802938968</v>
-      </c>
-      <c r="AR44" s="10">
-        <v>107598.92816371219</v>
-      </c>
-      <c r="AS44" s="10">
-        <v>119725.13696738242</v>
-      </c>
-      <c r="AT44" s="10">
-        <v>135055.88498327459</v>
-      </c>
-      <c r="AU44" s="10">
-        <v>142113.49627252799</v>
-      </c>
-      <c r="AV44" s="10">
-        <v>126257.99036284351</v>
-      </c>
-      <c r="AW44" s="10">
-        <v>126298.69954178153</v>
-      </c>
-      <c r="AX44" s="10">
-        <v>136884.81832356149</v>
-      </c>
-      <c r="AY44" s="10">
-        <v>146006.58336558813</v>
-      </c>
-      <c r="AZ44" s="10">
-        <v>143280.35475008565</v>
-      </c>
+      <c r="C44" s="14">
+        <v>112</v>
+      </c>
+      <c r="D44" s="14">
+        <v>118</v>
+      </c>
+      <c r="E44" s="14">
+        <v>131</v>
+      </c>
+      <c r="F44" s="14">
+        <v>156</v>
+      </c>
+      <c r="G44" s="14">
+        <v>159</v>
+      </c>
+      <c r="H44" s="14">
+        <v>176</v>
+      </c>
+      <c r="I44" s="14">
+        <v>163</v>
+      </c>
+      <c r="J44" s="14">
+        <v>183</v>
+      </c>
+      <c r="K44" s="14">
+        <v>225</v>
+      </c>
+      <c r="L44" s="14">
+        <v>267</v>
+      </c>
+      <c r="M44" s="14">
+        <v>306</v>
+      </c>
+      <c r="N44" s="14">
+        <v>286</v>
+      </c>
+      <c r="O44" s="14">
+        <v>276</v>
+      </c>
+      <c r="P44" s="14">
+        <v>292</v>
+      </c>
+      <c r="Q44" s="14">
+        <v>296</v>
+      </c>
+      <c r="R44" s="14">
+        <v>288</v>
+      </c>
+      <c r="S44" s="14">
+        <v>274</v>
+      </c>
+      <c r="T44" s="14">
+        <v>293</v>
+      </c>
+      <c r="U44" s="14">
+        <v>358</v>
+      </c>
+      <c r="V44" s="14">
+        <v>394</v>
+      </c>
+      <c r="W44" s="14">
+        <v>335</v>
+      </c>
+      <c r="X44" s="14">
+        <v>347</v>
+      </c>
+      <c r="Y44" s="14">
+        <v>409</v>
+      </c>
+      <c r="Z44" s="14">
+        <v>508</v>
+      </c>
+      <c r="AA44" s="14">
+        <v>459</v>
+      </c>
+      <c r="AB44" s="14">
+        <v>592</v>
+      </c>
+      <c r="AC44" s="14">
+        <v>690</v>
+      </c>
+      <c r="AD44" s="14">
+        <v>762</v>
+      </c>
+      <c r="AE44" s="14">
+        <v>809</v>
+      </c>
+      <c r="AF44" s="14">
+        <v>854</v>
+      </c>
+      <c r="AG44" s="14">
+        <v>939</v>
+      </c>
+      <c r="AH44" s="15">
+        <v>1031</v>
+      </c>
+      <c r="AI44" s="15">
+        <v>1125</v>
+      </c>
+      <c r="AJ44" s="15">
+        <v>1262</v>
+      </c>
+      <c r="AK44" s="15">
+        <v>1478</v>
+      </c>
+      <c r="AL44" s="15">
+        <v>1718</v>
+      </c>
+      <c r="AM44" s="15">
+        <v>2056</v>
+      </c>
+      <c r="AN44" s="15">
+        <v>2638</v>
+      </c>
+      <c r="AO44" s="15">
+        <v>3394</v>
+      </c>
+      <c r="AP44" s="15">
+        <v>3748</v>
+      </c>
+      <c r="AQ44" s="15">
+        <v>4447</v>
+      </c>
+      <c r="AR44" s="15">
+        <v>5486</v>
+      </c>
+      <c r="AS44" s="15">
+        <v>6164</v>
+      </c>
+      <c r="AT44" s="15">
+        <v>6876</v>
+      </c>
+      <c r="AU44" s="15">
+        <v>7486</v>
+      </c>
+      <c r="AV44" s="15">
+        <v>7863</v>
+      </c>
+      <c r="AW44" s="15">
+        <v>7944</v>
+      </c>
+      <c r="AX44" s="15">
+        <v>8663</v>
+      </c>
+      <c r="AY44" s="15">
+        <v>9733</v>
+      </c>
+      <c r="AZ44" s="16">
+        <v>10004</v>
+      </c>
+      <c r="BA44" s="13"/>
     </row>
-    <row r="45" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>170</v>
       </c>
@@ -8341,7 +8358,7 @@
         <v>6432.3875833954498</v>
       </c>
     </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>174</v>
       </c>
@@ -8499,7 +8516,7 @@
         <v>1370.1491682228411</v>
       </c>
     </row>
-    <row r="47" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>178</v>
       </c>
@@ -8657,7 +8674,7 @@
         <v>2304.126507736542</v>
       </c>
     </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>184</v>
       </c>
@@ -35121,21 +35138,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007024F25E6497ED43898D504973DBDCA9" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1bff820ca0c398a5b425d0da7d5a5f16">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4f447018-c40e-40e5-80f8-c919516cf764" xmlns:ns3="6b41ce5a-22ff-4aef-bca2-14b56bf0aa25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1a8e40961e45f55f365c0ad412ce4d6" ns2:_="" ns3:_="">
     <xsd:import namespace="4f447018-c40e-40e5-80f8-c919516cf764"/>
@@ -35352,24 +35354,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBE8A03E-93D3-4C95-817E-823E5A80B98B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8709A231-C639-4235-9C2D-B689DA930CED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C94D411D-FF49-470A-873E-89570DCD86EB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35386,4 +35386,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8709A231-C639-4235-9C2D-B689DA930CED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBE8A03E-93D3-4C95-817E-823E5A80B98B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>